<commit_message>
Small fixes to Matlab impl and added Matlab 2020 support.
</commit_message>
<xml_diff>
--- a/Matlab/Simulation/PortfolioData.xlsx
+++ b/Matlab/Simulation/PortfolioData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.liu.se\home\chred146\exjobb\MSc-Financial-Mathematics-Multi-Curve-Modeling-Risk-Performance-Attribution\TermStructureSimulation\MatlabTestSim\Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\MSc Git\MScCurveModeling\Matlab\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA066CD-7CDA-48AD-AFB6-90F91E362E68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFA426B-A094-475F-A304-CA30D529C282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2100" windowWidth="17490" windowHeight="8100" firstSheet="13" activeTab="16" xr2:uid="{1F1B9D4F-890A-446C-86EA-5F556401DAED}"/>
+    <workbookView xWindow="0" yWindow="2100" windowWidth="17490" windowHeight="8100" activeTab="6" xr2:uid="{1F1B9D4F-890A-446C-86EA-5F556401DAED}"/>
   </bookViews>
   <sheets>
     <sheet name="Float Cashflows EUR" sheetId="1" r:id="rId1"/>
@@ -284,290 +284,290 @@
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{072ED794-0A7F-409C-B89D-F95D14FE7CF0}_x0000_</stp>
+        <stp>{CED02AB9-17AE-48E9-B752-94414DBCA4CE}_x0000_</stp>
+        <tr r="AI6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{16706AA2-D7F6-4816-9122-AFAF2C01E536}_x0000_</stp>
+        <tr r="AE6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{786FDC0D-020F-4FE4-BEF9-034EACBA7D65}_x0000_</stp>
+        <tr r="AA6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{6737D2C5-4FC6-485D-B453-222FDDFC9F09}_x0000_</stp>
+        <tr r="W6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{8F3C3C57-22E0-42A7-B90E-E8EA579A95FF}_x0000_</stp>
+        <tr r="U6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{D74AB022-0090-4EC6-B296-E7FF91050869}_x0000_</stp>
+        <tr r="AA6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{FB320826-5272-4D71-B89A-938A0714654F}_x0000_</stp>
+        <tr r="AE6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{00065BA1-A1F1-4D03-9D85-14C74012C768}_x0000_</stp>
+        <tr r="AG6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{147887B2-0E93-46D1-A66F-562B588614C0}_x0000_</stp>
+        <tr r="X6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{E4DA37CD-FA96-4711-9F58-824D4AB7AB0C}_x0000_</stp>
+        <tr r="AD6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{FA9A1080-CBEF-42E4-B87A-20C8A83DA265}_x0000_</stp>
+        <tr r="AB6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{C8E950E9-7C7C-4087-AEE3-A6FE9656BE68}_x0000_</stp>
+        <tr r="AB6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{65157834-9868-4A9E-9E16-7CD1815CFBE0}_x0000_</stp>
+        <tr r="S6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{37791940-2D0E-4028-B9BF-1910E4256A5B}_x0000_</stp>
+        <tr r="Y6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{0B4C63E8-C307-46A6-BCB4-4845EAFCD9BF}_x0000_</stp>
+        <tr r="AC6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{711A2803-D0BC-4C09-876E-EA8A9D75DC16}_x0000_</stp>
+        <tr r="AD6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{5E0F8BB1-39CD-43C5-BE62-89429AB8DF0F}_x0000_</stp>
+        <tr r="V6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{4E7E54CD-7FF9-4D56-8D80-6DBC83A0ED3A}_x0000_</stp>
+        <tr r="AE6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{02A019F3-3627-4652-9E51-0E84BDD59457}_x0000_</stp>
+        <tr r="W6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{949E539F-F182-4D17-AD31-CB0F8D265EBF}_x0000_</stp>
+        <tr r="R6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{E6AD24E8-90DC-43D0-ACEC-3D81DFF6730F}_x0000_</stp>
+        <tr r="AD6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{6F06F322-E69A-469C-AE11-8EE4C4D6253C}_x0000_</stp>
+        <tr r="AH6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{41C31A6C-36BB-4176-9031-706A60C4996E}_x0000_</stp>
+        <tr r="W6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{07687C65-7F3B-4A78-ADCA-2F446EABB7BB}_x0000_</stp>
         <tr r="U6" s="13"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{B4699673-B6A5-4FD5-8CA7-F2ADA181386D}_x0000_</stp>
-        <tr r="AH6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{5B155B84-1415-43EB-8CFA-1CB40132DA89}_x0000_</stp>
-        <tr r="AE6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{61F1A2A3-DDC0-436F-9A35-5039052A5DD7}_x0000_</stp>
+        <stp>{6E1962B1-F0EB-4A2C-8716-5F94262099DE}_x0000_</stp>
         <tr r="AG6" s="3"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{7E3E8CB7-968E-40A4-A8FD-F7D623D97903}_x0000_</stp>
-        <tr r="AC6" s="3"/>
+        <stp>{F78406C0-2805-4777-BCC9-61D4122CD66B}_x0000_</stp>
+        <tr r="V6" s="13"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{8986890F-E08C-43B8-A23C-E2F99626E8D2}_x0000_</stp>
-        <tr r="T6" s="13"/>
+        <stp>{2E26701A-6075-4768-A8C0-06BEC7BECBDB}_x0000_</stp>
+        <tr r="Z6" s="12"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{08A7E0C8-F153-49A7-BEA9-EC9C6C6C102F}_x0000_</stp>
+        <stp>{3A8B27DE-9C34-47C0-8DDF-61BF3B693AA0}_x0000_</stp>
+        <tr r="AH6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{AC373043-FAC7-407C-AAD9-D1C00D15F11D}_x0000_</stp>
+        <tr r="Y6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{401A4FDA-3EFE-4918-870D-AE573AA2AEA3}_x0000_</stp>
+        <tr r="Z6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{0847B1D2-FE4C-4405-BDBE-F52269ABDF5F}_x0000_</stp>
+        <tr r="U6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{9AA581BE-3E86-4E09-B206-14C7E4C03D69}_x0000_</stp>
+        <tr r="AG6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{EBA91BB5-973C-47BC-9976-ACE398A181DB}_x0000_</stp>
+        <tr r="X6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{B1DE85B8-B345-4ACA-86EA-8D442E4C2616}_x0000_</stp>
+        <tr r="AA6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{BA99A7DB-B992-4BEE-A691-04A52050CA04}_x0000_</stp>
+        <tr r="AF6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{E592405C-02A3-4A5F-A4A7-252D23350F22}_x0000_</stp>
+        <tr r="T6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{9CDB0C36-9AC7-449D-B7F0-7C63A9907940}_x0000_</stp>
+        <tr r="AF6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{629C0A4E-9E5E-427F-9A19-290B2890D1A8}_x0000_</stp>
+        <tr r="AC6" s="13"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{6861847F-1DC3-49B9-A94B-344276407143}_x0000_</stp>
+        <tr r="Y6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{A315597E-445E-4173-90B5-F30FD79A5EA7}_x0000_</stp>
+        <tr r="AC6" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{EBDE697A-D6AA-4342-983B-C332EC21B8B0}_x0000_</stp>
+        <tr r="AB6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{01642EE4-A0CE-4FCB-B082-E4D884BABFDA}_x0000_</stp>
+        <tr r="V6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{27B1AC8F-77E1-421F-9313-6AA0D98131BA}_x0000_</stp>
+        <tr r="Z6" s="3"/>
+      </tp>
+      <tp t="s">
+        <v>Not Signed In</v>
+        <stp/>
+        <stp>{0CBD6165-F75C-494B-A9A7-490432C2710B}_x0000_</stp>
         <tr r="AF6" s="3"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{0769BEB8-DC9B-4CB9-AA23-872D3BD9AE0A}_x0000_</stp>
-        <tr r="T6" s="12"/>
+        <stp>{9B697010-F0BD-411E-B5DC-3856139F9E60}_x0000_</stp>
+        <tr r="S6" s="13"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{2362B1A2-ADFC-48C4-902B-C86D7E65A650}_x0000_</stp>
-        <tr r="AB6" s="12"/>
+        <stp>{48215CD5-928C-4BA2-BE86-7AC560AD6A45}_x0000_</stp>
+        <tr r="T6" s="3"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{FD48C05A-25D5-4435-A554-E2A6E6DA5A89}_x0000_</stp>
-        <tr r="AA6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{D7344B27-3ACA-4762-8DD1-96956D5885DC}_x0000_</stp>
-        <tr r="Z6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{3DC6B9B0-ED5E-44A7-8474-080867F71CF1}_x0000_</stp>
-        <tr r="AH6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{73D4D96B-FD33-4D7C-A673-1A53684D8C85}_x0000_</stp>
-        <tr r="W6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{5FF915E8-EE1A-45D9-A856-D7E93F2F3117}_x0000_</stp>
-        <tr r="AB6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{F4317C7E-9416-409E-9DF9-1534A05F6CC1}_x0000_</stp>
-        <tr r="X6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{D677081A-6624-45B6-9626-0AAEF2E43456}_x0000_</stp>
-        <tr r="AE6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{1A2E1975-87A0-4CD9-899F-79A5718EF975}_x0000_</stp>
+        <stp>{E4E92CCB-5EBA-4487-B285-C9E1216789C2}_x0000_</stp>
         <tr r="X6" s="3"/>
       </tp>
       <tp t="s">
         <v>Not Signed In</v>
         <stp/>
-        <stp>{911A3452-C4A4-4342-8A31-DEBCE18F3D22}_x0000_</stp>
-        <tr r="AG6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{F71F96B6-EF95-4A02-8E70-3FA5B509EDB2}_x0000_</stp>
-        <tr r="AD6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{F86739E3-A01B-41EC-9077-50B77A30B094}_x0000_</stp>
-        <tr r="T6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{86366FDE-618A-4708-9951-BBDF88927728}_x0000_</stp>
-        <tr r="Z6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{B863EE8A-C440-4590-9E0E-BFC761FAA3F4}_x0000_</stp>
-        <tr r="U6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{170DBF7F-561E-4406-8ABE-93D733196E99}_x0000_</stp>
-        <tr r="AF6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{201B565C-9D96-431B-9C4E-2F5816E51E57}_x0000_</stp>
-        <tr r="AC6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{37038A82-38BB-4F37-A84D-E24E2DF937B0}_x0000_</stp>
-        <tr r="AF6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{30B5423A-4512-46ED-92C5-D96716B6E8FA}_x0000_</stp>
-        <tr r="V6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{CF522C0F-2AE7-490F-A24B-B682D018FC77}_x0000_</stp>
-        <tr r="AD6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{316C337E-A2ED-4774-BF2B-0244569A2BE7}_x0000_</stp>
-        <tr r="AA6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{EA19C589-E063-402B-B69C-E3E73C47D650}_x0000_</stp>
-        <tr r="S6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{C8D7BBB7-983B-479A-A094-F92731217554}_x0000_</stp>
-        <tr r="Z6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{4FF78186-2A5D-4552-AB87-1732EFBA12DC}_x0000_</stp>
-        <tr r="AA6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{EA449CB9-8364-4DA7-8F79-3AC1C8E13F17}_x0000_</stp>
-        <tr r="AI6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{103568E9-8AB1-465E-BC68-3C7BC0C92D21}_x0000_</stp>
-        <tr r="U6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{1F655251-0E95-4398-85B1-333D16C147B0}_x0000_</stp>
-        <tr r="AB6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{EF231F38-339C-4B6F-9F79-2679ACF53F16}_x0000_</stp>
-        <tr r="R6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{B140B6D8-67E1-4647-85B9-1AE3592C287A}_x0000_</stp>
-        <tr r="AD6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{5FF4F1FB-C68A-4614-BCE6-0A70BFCFB123}_x0000_</stp>
-        <tr r="Y6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{89B22F4E-B9B9-4B13-8E57-244AB40C29C2}_x0000_</stp>
-        <tr r="AE6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{7AFCF0BC-1375-4B61-8476-063E2B47383A}_x0000_</stp>
-        <tr r="V6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{6EA9E2D4-6970-4989-A8C9-FE3639498893}_x0000_</stp>
-        <tr r="Y6" s="3"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{EC4DAC11-2F25-4A6E-BE86-6CA48467CCF9}_x0000_</stp>
-        <tr r="AG6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{9EC746A7-0436-403E-8582-62F432E7EFDA}_x0000_</stp>
-        <tr r="Y6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{86261000-61F8-4D18-968F-3564CECE2FA4}_x0000_</stp>
-        <tr r="W6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{96DD326A-A179-4498-9FF5-0FE1DC6F2730}_x0000_</stp>
-        <tr r="AC6" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{2EFC002E-3416-4549-83CD-DF9D989446E1}_x0000_</stp>
-        <tr r="W6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{DA3DE9B7-2330-48F7-8696-4740A45928B2}_x0000_</stp>
-        <tr r="V6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{A5190888-D72C-436C-8910-56B55E420DEE}_x0000_</stp>
-        <tr r="X6" s="13"/>
-      </tp>
-      <tp t="s">
-        <v>Not Signed In</v>
-        <stp/>
-        <stp>{29D30250-9A47-4950-AA0E-6C62C4824ED5}_x0000_</stp>
-        <tr r="S6" s="13"/>
+        <stp>{CB188FC2-9D12-4160-B5B4-83120B6299A2}_x0000_</stp>
+        <tr r="T6" s="13"/>
       </tp>
     </main>
   </volType>
@@ -32849,7 +32849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB49B52A-17B6-47F8-AC54-B3BF97D638EF}">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
@@ -44432,7 +44432,7 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44868,7 +44868,7 @@
   <dimension ref="A1:AI19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N11"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -60719,7 +60719,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61708,8 +61708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978A1691-C04C-4179-90DE-9F6AAF02DD5B}">
   <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -72698,7 +72698,7 @@
   <dimension ref="A1:AI534"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -90448,8 +90448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506B553D-9EC9-440F-B473-4E2B6BD83CE9}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>